<commit_message>
MTF 2013 8/10grade group creation
</commit_message>
<xml_diff>
--- a/PATH/Kim Invoice Rubric.xlsx
+++ b/PATH/Kim Invoice Rubric.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t>Process 2000-2019 MTF data to create youth groups on life expectations, future plans, etc.</t>
+  </si>
+  <si>
+    <t>Factor Analysis for 2013 MTF future outlook, social media, parental background groups</t>
   </si>
 </sst>
 </file>
@@ -573,7 +576,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -880,11 +883,20 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B23" s="15"/>
-      <c r="C23"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="7"/>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="B23" s="15">
+        <v>44172</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="E23" s="7">
+        <f t="shared" ref="E23" si="7">D23*40</f>
+        <v>100</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B24" s="15"/>
@@ -922,7 +934,7 @@
       </c>
       <c r="E29" s="8">
         <f>SUM(E5:E27)</f>
-        <v>1220</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
first commit webs crape script
</commit_message>
<xml_diff>
--- a/PATH/Kim Invoice Rubric.xlsx
+++ b/PATH/Kim Invoice Rubric.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -125,6 +125,12 @@
   </si>
   <si>
     <t>Factor Analysis for 2013 MTF future outlook, social media, parental background groups</t>
+  </si>
+  <si>
+    <t>Clean up 2013 8/10th MTF data for FA and figure out NA issue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clean ALL years MTF data for FA </t>
   </si>
 </sst>
 </file>
@@ -576,7 +582,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -885,7 +891,7 @@
     </row>
     <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="B23" s="15">
-        <v>44172</v>
+        <v>44173</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>27</v>
@@ -899,16 +905,34 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B24" s="15"/>
-      <c r="C24"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="7"/>
+      <c r="B24" s="15">
+        <v>44174</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="18">
+        <v>2</v>
+      </c>
+      <c r="E24" s="7">
+        <f t="shared" ref="E24" si="8">D24*40</f>
+        <v>80</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B25" s="15"/>
-      <c r="C25"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="7"/>
+      <c r="B25" s="15">
+        <v>44175</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="18">
+        <v>1</v>
+      </c>
+      <c r="E25" s="7">
+        <f t="shared" ref="E25" si="9">D25*40</f>
+        <v>40</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B26" s="15"/>
@@ -934,7 +958,7 @@
       </c>
       <c r="E29" s="8">
         <f>SUM(E5:E27)</f>
-        <v>1320</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>